<commit_message>
Added export PDF and Word to all Reports.
Will need to test them all once data is inputted. Some reports had no data so I was not able to test them.
</commit_message>
<xml_diff>
--- a/src/SFA/wwwroot/resources/reports/User Activity Report.xlsx
+++ b/src/SFA/wwwroot/resources/reports/User Activity Report.xlsx
@@ -23,7 +23,7 @@
     <t>Report Generation Date &amp; Time :</t>
   </si>
   <si>
-    <t>04-12-2022</t>
+    <t>06-12-2022</t>
   </si>
   <si>
     <t>Report Generated By :</t>
@@ -68,7 +68,7 @@
     <t>LOG IN</t>
   </si>
   <si>
-    <t>04-12-2022 14:23:48</t>
+    <t>06-12-2022 10:15:18</t>
   </si>
   <si>
     <t>CHURCH</t>

</xml_diff>

<commit_message>
Added email send for missionary on approved Macro and added 1C email template for email to DGMD on macro insert
</commit_message>
<xml_diff>
--- a/src/SFA/wwwroot/resources/reports/User Activity Report.xlsx
+++ b/src/SFA/wwwroot/resources/reports/User Activity Report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>UPCI GLOBAL MISSIONS DEPUTATION MANAGEMENT SYSTEM.</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Report Generation Date &amp; Time :</t>
   </si>
   <si>
-    <t>06-12-2022</t>
+    <t>23-01-2023</t>
   </si>
   <si>
     <t>Report Generated By :</t>
@@ -62,43 +62,85 @@
     <t>admin@contezza.in</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>LOG IN</t>
-  </si>
-  <si>
-    <t>06-12-2022 10:15:18</t>
-  </si>
-  <si>
-    <t>CHURCH</t>
-  </si>
-  <si>
-    <t>Take2</t>
-  </si>
-  <si>
-    <t>CHURCH CREATE</t>
-  </si>
-  <si>
-    <t>04-12-2022 12:43:29</t>
-  </si>
-  <si>
-    <t>TestNTA</t>
-  </si>
-  <si>
-    <t>CHURCH UPDATE</t>
-  </si>
-  <si>
-    <t>04-12-2022 12:28:46</t>
-  </si>
-  <si>
-    <t>04-12-2022 12:20:29</t>
-  </si>
-  <si>
-    <t>NTAAlabamaChurch2</t>
-  </si>
-  <si>
-    <t>03-12-2022 21:19:19</t>
+    <t>APPOINTMENT</t>
+  </si>
+  <si>
+    <t>This is going well.</t>
+  </si>
+  <si>
+    <t>APPOINTMENT CREATE</t>
+  </si>
+  <si>
+    <t>13-01-2023 11:40:16</t>
+  </si>
+  <si>
+    <t>MACRO SCHEDULE</t>
+  </si>
+  <si>
+    <t>f34f4f34f FOR Michigan</t>
+  </si>
+  <si>
+    <t>MACRO SCHEDULE CREATE</t>
+  </si>
+  <si>
+    <t>06-01-2023 08:43:21</t>
+  </si>
+  <si>
+    <t>yttyyty FOR Michigan</t>
+  </si>
+  <si>
+    <t>06-01-2023 08:35:48</t>
+  </si>
+  <si>
+    <t>ffff FOR Michigan</t>
+  </si>
+  <si>
+    <t>06-01-2023 08:32:08</t>
+  </si>
+  <si>
+    <t>Testing email for Troy as DGMD FOR Michigan</t>
+  </si>
+  <si>
+    <t>04-01-2023 19:18:08</t>
+  </si>
+  <si>
+    <t>Test Email Troy FOR Alabama</t>
+  </si>
+  <si>
+    <t>04-01-2023 16:33:48</t>
+  </si>
+  <si>
+    <t>Testing email FOR Washington</t>
+  </si>
+  <si>
+    <t>04-01-2023 16:17:42</t>
+  </si>
+  <si>
+    <t>APPOINTMENT ACCEPT BY PASTOR</t>
+  </si>
+  <si>
+    <t>03-01-2023 21:53:54</t>
+  </si>
+  <si>
+    <t>APPOINTMENT SUBMIT</t>
+  </si>
+  <si>
+    <t>03-01-2023 21:50:55</t>
+  </si>
+  <si>
+    <t>03-01-2023 21:49:30</t>
+  </si>
+  <si>
+    <t>CHURCH SERVICE TIME</t>
+  </si>
+  <si>
+    <t>NTAAlabamaChurch2 FOR Monday</t>
+  </si>
+  <si>
+    <t>CHURCH SERVICE TIME CREATE</t>
+  </si>
+  <si>
+    <t>03-01-2023 13:35:58</t>
   </si>
 </sst>
 </file>
@@ -174,7 +216,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -261,13 +303,13 @@
         <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
@@ -284,16 +326,16 @@
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -310,13 +352,13 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>25</v>
@@ -336,16 +378,16 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
@@ -362,16 +404,172 @@
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Code Fixes and Existing Code enhacnemnts
API Check for Adding data with addresses.
Code for 2 week automation email
Small big fixes that were mentioned on Monday Board
</commit_message>
<xml_diff>
--- a/src/SFA/wwwroot/resources/reports/User Activity Report.xlsx
+++ b/src/SFA/wwwroot/resources/reports/User Activity Report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>UPCI GLOBAL MISSIONS DEPUTATION MANAGEMENT SYSTEM.</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Report Generation Date &amp; Time :</t>
   </si>
   <si>
-    <t>23-01-2023</t>
+    <t>17-02-2023</t>
   </si>
   <si>
     <t>Report Generated By :</t>
@@ -65,82 +65,64 @@
     <t>APPOINTMENT</t>
   </si>
   <si>
+    <t>dwewcd</t>
+  </si>
+  <si>
+    <t>APPOINTMENT CREATE</t>
+  </si>
+  <si>
+    <t>10-02-2023 08:06:41</t>
+  </si>
+  <si>
     <t>This is going well.</t>
   </si>
   <si>
-    <t>APPOINTMENT CREATE</t>
-  </si>
-  <si>
-    <t>13-01-2023 11:40:16</t>
-  </si>
-  <si>
-    <t>MACRO SCHEDULE</t>
-  </si>
-  <si>
-    <t>f34f4f34f FOR Michigan</t>
-  </si>
-  <si>
-    <t>MACRO SCHEDULE CREATE</t>
-  </si>
-  <si>
-    <t>06-01-2023 08:43:21</t>
-  </si>
-  <si>
-    <t>yttyyty FOR Michigan</t>
-  </si>
-  <si>
-    <t>06-01-2023 08:35:48</t>
-  </si>
-  <si>
-    <t>ffff FOR Michigan</t>
-  </si>
-  <si>
-    <t>06-01-2023 08:32:08</t>
-  </si>
-  <si>
-    <t>Testing email for Troy as DGMD FOR Michigan</t>
-  </si>
-  <si>
-    <t>04-01-2023 19:18:08</t>
-  </si>
-  <si>
-    <t>Test Email Troy FOR Alabama</t>
-  </si>
-  <si>
-    <t>04-01-2023 16:33:48</t>
-  </si>
-  <si>
-    <t>Testing email FOR Washington</t>
-  </si>
-  <si>
-    <t>04-01-2023 16:17:42</t>
+    <t>10-02-2023 08:05:26</t>
+  </si>
+  <si>
+    <t>10-02-2023 08:04:32</t>
+  </si>
+  <si>
+    <t>APPOINTMENT SUBMIT</t>
+  </si>
+  <si>
+    <t>10-02-2023 07:28:16</t>
+  </si>
+  <si>
+    <t>10-02-2023 07:20:27</t>
+  </si>
+  <si>
+    <t>09-02-2023 21:48:00</t>
+  </si>
+  <si>
+    <t>09-02-2023 21:44:02</t>
+  </si>
+  <si>
+    <t>09-02-2023 21:28:19</t>
+  </si>
+  <si>
+    <t>09-02-2023 21:27:11</t>
+  </si>
+  <si>
+    <t>09-02-2023 21:25:21</t>
   </si>
   <si>
     <t>APPOINTMENT ACCEPT BY PASTOR</t>
   </si>
   <si>
-    <t>03-01-2023 21:53:54</t>
-  </si>
-  <si>
-    <t>APPOINTMENT SUBMIT</t>
-  </si>
-  <si>
-    <t>03-01-2023 21:50:55</t>
-  </si>
-  <si>
-    <t>03-01-2023 21:49:30</t>
-  </si>
-  <si>
-    <t>CHURCH SERVICE TIME</t>
-  </si>
-  <si>
-    <t>NTAAlabamaChurch2 FOR Monday</t>
-  </si>
-  <si>
-    <t>CHURCH SERVICE TIME CREATE</t>
-  </si>
-  <si>
-    <t>03-01-2023 13:35:58</t>
+    <t>09-02-2023 21:24:31</t>
+  </si>
+  <si>
+    <t>09-02-2023 21:23:58</t>
+  </si>
+  <si>
+    <t>newwwww</t>
+  </si>
+  <si>
+    <t>09-02-2023 20:26:22</t>
+  </si>
+  <si>
+    <t>07-02-2023 23:38:01</t>
   </si>
 </sst>
 </file>
@@ -216,7 +198,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -326,16 +308,16 @@
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -352,16 +334,16 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -378,16 +360,16 @@
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
@@ -404,16 +386,16 @@
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
@@ -430,16 +412,16 @@
         <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
@@ -456,16 +438,16 @@
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
@@ -485,13 +467,13 @@
         <v>16</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
@@ -511,13 +493,13 @@
         <v>16</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
@@ -537,13 +519,13 @@
         <v>16</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15">
@@ -560,16 +542,146 @@
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>